<commit_message>
started changing result matrices from 16 to 8 lines
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\matlab-mltool-fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC886947-77F6-4030-9C2F-B2B1AD281ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F179EFD7-7265-4EC1-8890-060A016617DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="32">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -529,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -727,6 +727,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1012,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1621,7 @@
         <v>0.913333333333333</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -1607,96 +1631,164 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D29" s="16"/>
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -1941,7 +2033,7 @@
   <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3287,10 +3379,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8065C56F-AEED-4D36-9CB5-AF6203A45422}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3880,6 +3972,168 @@
         <v>0.78849448737398597</v>
       </c>
     </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
@@ -3890,10 +4144,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF1E589-1659-439B-B1DA-4F9E028A9755}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4483,6 +4737,168 @@
         <v>0.89045134120662806</v>
       </c>
     </row>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
@@ -4495,8 +4911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BD5FD7-7F47-465E-A9A3-1FAE665B7AD8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5080,7 +5496,7 @@
         <v>1.4134664138513E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -5090,96 +5506,164 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D29" s="16"/>
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -5424,7 +5908,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6008,8 +6492,165 @@
         <v>0.91537132987910197</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -6194,7 +6835,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6778,7 +7419,7 @@
         <v>0.94645941278065604</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
@@ -6788,96 +7429,164 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D29" s="16"/>
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -7122,7 +7831,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7706,8 +8415,165 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -7892,7 +8758,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8476,8 +9342,165 @@
         <v>125.82</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -8662,7 +9685,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9246,8 +10269,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -9432,7 +10612,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10016,8 +11196,165 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="69"/>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="72"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="69"/>
+    </row>
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="70"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="72"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="69"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="72"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="74"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -10202,7 +11539,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added reduced matrices of results for CC, VC and WF
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\matlab-mltool-fp\results_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F179EFD7-7265-4EC1-8890-060A016617DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D07E79-9012-4CCD-8B55-5EAFF121ECC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -711,24 +711,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -751,6 +733,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,19 +1055,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1672,28 +1672,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>0.87633851468048396</v>
+      </c>
+      <c r="E23" s="62">
+        <v>0.89400690846286701</v>
+      </c>
+      <c r="F23" s="62">
+        <v>0.89162348877374797</v>
+      </c>
+      <c r="G23" s="62">
+        <v>0.82811744386873898</v>
+      </c>
+      <c r="H23" s="62">
+        <v>0.83075993091537104</v>
+      </c>
+      <c r="I23" s="62">
+        <v>0.90312607944732304</v>
+      </c>
+      <c r="J23" s="62">
+        <v>0.88198618307426602</v>
+      </c>
+      <c r="K23" s="63">
+        <v>0.803920552677029</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>0.89388601036269399</v>
+      </c>
+      <c r="E24" s="65">
+        <v>0.85602763385146796</v>
+      </c>
+      <c r="F24" s="65">
+        <v>0.85670120898100199</v>
+      </c>
+      <c r="G24" s="65">
+        <v>0.81253886010362697</v>
+      </c>
+      <c r="H24" s="65">
+        <v>0.80283246977547496</v>
+      </c>
+      <c r="I24" s="65">
+        <v>0.938791018998273</v>
+      </c>
+      <c r="J24" s="65">
+        <v>0.90037996545768595</v>
+      </c>
+      <c r="K24" s="66">
+        <v>0.88943005181347201</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -1703,28 +1735,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>0.90373056994818701</v>
+      </c>
+      <c r="E25" s="62">
+        <v>0.76649395509499096</v>
+      </c>
+      <c r="F25" s="62">
+        <v>0.90469775474956804</v>
+      </c>
+      <c r="G25" s="62">
+        <v>0.87523316062176204</v>
+      </c>
+      <c r="H25" s="62">
+        <v>0.87853195164076003</v>
+      </c>
+      <c r="I25" s="62">
+        <v>0.92369602763385195</v>
+      </c>
+      <c r="J25" s="62">
+        <v>0.91958549222797903</v>
+      </c>
+      <c r="K25" s="63">
+        <v>0.82728842832469796</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>0.90796200345423095</v>
+      </c>
+      <c r="E26" s="65">
+        <v>0.87051813471502604</v>
+      </c>
+      <c r="F26" s="65">
+        <v>0.78340241796200405</v>
+      </c>
+      <c r="G26" s="65">
+        <v>0.79815198618307404</v>
+      </c>
+      <c r="H26" s="65">
+        <v>0.76785837651122602</v>
+      </c>
+      <c r="I26" s="65">
+        <v>0.90302245250431801</v>
+      </c>
+      <c r="J26" s="65">
+        <v>0.90390328151986199</v>
+      </c>
+      <c r="K26" s="66">
+        <v>0.83473229706390295</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1734,14 +1798,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>0.81202072538860104</v>
+      </c>
+      <c r="E27" s="62">
+        <v>0.86215889464594098</v>
+      </c>
+      <c r="F27" s="62">
+        <v>0.87861830742659797</v>
+      </c>
+      <c r="G27" s="62">
+        <v>0.81649395509499101</v>
+      </c>
+      <c r="H27" s="62">
+        <v>0.84929188255613097</v>
+      </c>
+      <c r="I27" s="62">
+        <v>0.87062176165803096</v>
+      </c>
+      <c r="J27" s="62">
+        <v>0.85457685664939498</v>
+      </c>
+      <c r="K27" s="63">
+        <v>0.88113989637305701</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -1749,14 +1829,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>0.87278065630397195</v>
+      </c>
+      <c r="E28" s="65">
+        <v>0.84659758203799695</v>
+      </c>
+      <c r="F28" s="65">
+        <v>0.84785837651122598</v>
+      </c>
+      <c r="G28" s="65">
+        <v>0.84816925734024196</v>
+      </c>
+      <c r="H28" s="65">
+        <v>0.84350604490500902</v>
+      </c>
+      <c r="I28" s="65">
+        <v>0.81155440414507796</v>
+      </c>
+      <c r="J28" s="65">
+        <v>0.78910189982728796</v>
+      </c>
+      <c r="K28" s="66">
+        <v>0.86214162348877399</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -1766,14 +1862,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>0.92203799654576901</v>
+      </c>
+      <c r="E29" s="16">
+        <v>0.51495682210708105</v>
+      </c>
+      <c r="F29" s="16">
+        <v>0.89070811744386902</v>
+      </c>
+      <c r="G29" s="16">
+        <v>0.91837651122625197</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.91870466321243505</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0.61965457685665004</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0.819084628670121</v>
+      </c>
+      <c r="K29" s="68">
+        <v>0.90528497409326403</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -1781,14 +1893,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>0.92295336787564797</v>
+      </c>
+      <c r="E30" s="65">
+        <v>0.903747841105354</v>
+      </c>
+      <c r="F30" s="65">
+        <v>0.89053540587219304</v>
+      </c>
+      <c r="G30" s="65">
+        <v>0.90041450777202103</v>
+      </c>
+      <c r="H30" s="65">
+        <v>0.89150259067357496</v>
+      </c>
+      <c r="I30" s="65">
+        <v>0.76082901554404103</v>
+      </c>
+      <c r="J30" s="65">
+        <v>0.84428324697754698</v>
+      </c>
+      <c r="K30" s="66">
+        <v>0.913333333333333</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -2054,61 +2182,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="64"/>
-      <c r="F3" s="63" t="s">
+      <c r="E3" s="72"/>
+      <c r="F3" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="64"/>
-      <c r="H3" s="63" t="s">
+      <c r="G3" s="72"/>
+      <c r="H3" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="63" t="s">
+      <c r="I3" s="72"/>
+      <c r="J3" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="64"/>
-      <c r="L3" s="63" t="s">
+      <c r="K3" s="72"/>
+      <c r="L3" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="63" t="s">
+      <c r="M3" s="72"/>
+      <c r="N3" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="64"/>
-      <c r="P3" s="63" t="s">
+      <c r="O3" s="72"/>
+      <c r="P3" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="63" t="s">
+      <c r="Q3" s="72"/>
+      <c r="R3" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="65"/>
+      <c r="S3" s="73"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -3393,19 +3521,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4014,14 +4142,14 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
@@ -4029,14 +4157,14 @@
         <v>2</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -4046,14 +4174,14 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -4061,14 +4189,14 @@
         <v>2</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -4078,14 +4206,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -4093,14 +4221,14 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -4110,14 +4238,14 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="K29" s="68"/>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -4125,14 +4253,14 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4158,19 +4286,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4779,14 +4907,14 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
@@ -4794,14 +4922,14 @@
         <v>2</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -4811,14 +4939,14 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
@@ -4826,14 +4954,14 @@
         <v>2</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -4843,14 +4971,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -4858,14 +4986,14 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -4875,14 +5003,14 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="K29" s="68"/>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -4890,14 +5018,14 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4912,7 +5040,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4930,19 +5058,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5547,28 +5675,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>5.31511466683064E-2</v>
+      </c>
+      <c r="E23" s="62">
+        <v>6.13883782872277E-2</v>
+      </c>
+      <c r="F23" s="62">
+        <v>5.5288075112571798E-2</v>
+      </c>
+      <c r="G23" s="62">
+        <v>8.2874465663765606E-2</v>
+      </c>
+      <c r="H23" s="62">
+        <v>7.0073905958158905E-2</v>
+      </c>
+      <c r="I23" s="62">
+        <v>0.120603182497484</v>
+      </c>
+      <c r="J23" s="62">
+        <v>8.6580908912160304E-2</v>
+      </c>
+      <c r="K23" s="63">
+        <v>0.101685806542979</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>6.3742683806126604E-2</v>
+      </c>
+      <c r="E24" s="65">
+        <v>6.9135429063993697E-2</v>
+      </c>
+      <c r="F24" s="65">
+        <v>6.1500575184756198E-2</v>
+      </c>
+      <c r="G24" s="65">
+        <v>0.15182758710626601</v>
+      </c>
+      <c r="H24" s="65">
+        <v>0.153690798183582</v>
+      </c>
+      <c r="I24" s="65">
+        <v>1.9854160776916398E-2</v>
+      </c>
+      <c r="J24" s="65">
+        <v>7.1925202741607602E-2</v>
+      </c>
+      <c r="K24" s="66">
+        <v>6.6403541208464603E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -5578,28 +5738,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>5.7715116480862201E-2</v>
+      </c>
+      <c r="E25" s="62">
+        <v>0.20847294749992501</v>
+      </c>
+      <c r="F25" s="62">
+        <v>3.8083974582962497E-2</v>
+      </c>
+      <c r="G25" s="62">
+        <v>5.9673790100597E-2</v>
+      </c>
+      <c r="H25" s="62">
+        <v>6.04009583224841E-2</v>
+      </c>
+      <c r="I25" s="62">
+        <v>1.13038317941467E-2</v>
+      </c>
+      <c r="J25" s="62">
+        <v>2.01479187856798E-2</v>
+      </c>
+      <c r="K25" s="63">
+        <v>9.6386443541113198E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>5.0015196315053599E-2</v>
+      </c>
+      <c r="E26" s="65">
+        <v>4.5722513237984798E-2</v>
+      </c>
+      <c r="F26" s="65">
+        <v>0.109093855948639</v>
+      </c>
+      <c r="G26" s="65">
+        <v>6.3086680279285101E-2</v>
+      </c>
+      <c r="H26" s="65">
+        <v>8.6553774186962903E-2</v>
+      </c>
+      <c r="I26" s="65">
+        <v>1.19339758707411E-2</v>
+      </c>
+      <c r="J26" s="65">
+        <v>1.3444501930131201E-2</v>
+      </c>
+      <c r="K26" s="66">
+        <v>6.5475819226124304E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -5609,14 +5801,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>8.1494591343471298E-2</v>
+      </c>
+      <c r="E27" s="62">
+        <v>5.4834605954378002E-2</v>
+      </c>
+      <c r="F27" s="62">
+        <v>3.1443760859088801E-2</v>
+      </c>
+      <c r="G27" s="62">
+        <v>0.123523660046651</v>
+      </c>
+      <c r="H27" s="62">
+        <v>2.6059943690663601E-2</v>
+      </c>
+      <c r="I27" s="62">
+        <v>4.3072109213126999E-2</v>
+      </c>
+      <c r="J27" s="62">
+        <v>5.7745586138065998E-2</v>
+      </c>
+      <c r="K27" s="63">
+        <v>2.8563947457094001E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -5624,14 +5832,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>2.94293564378529E-2</v>
+      </c>
+      <c r="E28" s="65">
+        <v>2.63219633167316E-2</v>
+      </c>
+      <c r="F28" s="65">
+        <v>2.5790864547530601E-2</v>
+      </c>
+      <c r="G28" s="65">
+        <v>2.3636564444323702E-2</v>
+      </c>
+      <c r="H28" s="65">
+        <v>2.8969832718920199E-2</v>
+      </c>
+      <c r="I28" s="65">
+        <v>0.18298848176138999</v>
+      </c>
+      <c r="J28" s="65">
+        <v>0.169423329517192</v>
+      </c>
+      <c r="K28" s="66">
+        <v>2.5549404381787402E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -5641,14 +5865,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>3.2039826872185498E-2</v>
+      </c>
+      <c r="E29" s="16">
+        <v>0.37550353155308802</v>
+      </c>
+      <c r="F29" s="16">
+        <v>2.3425267963234998E-2</v>
+      </c>
+      <c r="G29" s="16">
+        <v>1.3131816881986801E-2</v>
+      </c>
+      <c r="H29" s="16">
+        <v>1.17042317994636E-2</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0.35604358198722602</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0.19879933694117399</v>
+      </c>
+      <c r="K29" s="68">
+        <v>1.8628668661975101E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -5656,14 +5896,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>2.5913009597208998E-2</v>
+      </c>
+      <c r="E30" s="65">
+        <v>1.24878825699428E-2</v>
+      </c>
+      <c r="F30" s="65">
+        <v>4.4413696083633297E-2</v>
+      </c>
+      <c r="G30" s="65">
+        <v>1.2210627798266999E-2</v>
+      </c>
+      <c r="H30" s="65">
+        <v>4.3943513039942497E-2</v>
+      </c>
+      <c r="I30" s="65">
+        <v>0.20555535272363301</v>
+      </c>
+      <c r="J30" s="65">
+        <v>0.15345123830844901</v>
+      </c>
+      <c r="K30" s="66">
+        <v>1.4134664138513E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -5926,19 +6182,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6534,28 +6790,28 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -6565,28 +6821,28 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -6596,14 +6852,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -6611,14 +6867,14 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -6628,14 +6884,14 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="K29" s="68"/>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -6643,14 +6899,14 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -6853,19 +7109,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7470,28 +7726,28 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="63"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="66"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -7501,28 +7757,28 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="63"/>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="66"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -7532,14 +7788,14 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="63"/>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -7547,14 +7803,14 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="66"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -7564,14 +7820,14 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="16"/>
       <c r="H29" s="16"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="K29" s="68"/>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -7579,14 +7835,14 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="66"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D31" s="16"/>
@@ -7831,7 +8087,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7839,29 +8095,26 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8457,28 +8710,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>25</v>
+      </c>
+      <c r="E23" s="62">
+        <v>53</v>
+      </c>
+      <c r="F23" s="62">
+        <v>41</v>
+      </c>
+      <c r="G23" s="62">
+        <v>38</v>
+      </c>
+      <c r="H23" s="62">
+        <v>42</v>
+      </c>
+      <c r="I23" s="62">
+        <v>270</v>
+      </c>
+      <c r="J23" s="62">
+        <v>10</v>
+      </c>
+      <c r="K23" s="63">
+        <v>19</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>19</v>
+      </c>
+      <c r="E24" s="65">
+        <v>29</v>
+      </c>
+      <c r="F24" s="65">
+        <v>21</v>
+      </c>
+      <c r="G24" s="65">
+        <v>17</v>
+      </c>
+      <c r="H24" s="65">
+        <v>14</v>
+      </c>
+      <c r="I24" s="65">
+        <v>89</v>
+      </c>
+      <c r="J24" s="65">
+        <v>15</v>
+      </c>
+      <c r="K24" s="66">
+        <v>36</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -8488,28 +8773,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>19</v>
+      </c>
+      <c r="E25" s="62">
+        <v>6</v>
+      </c>
+      <c r="F25" s="62">
+        <v>88</v>
+      </c>
+      <c r="G25" s="62">
+        <v>52</v>
+      </c>
+      <c r="H25" s="62">
+        <v>45</v>
+      </c>
+      <c r="I25" s="62">
+        <v>270</v>
+      </c>
+      <c r="J25" s="62">
+        <v>53</v>
+      </c>
+      <c r="K25" s="63">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>19</v>
+      </c>
+      <c r="E26" s="65">
+        <v>33</v>
+      </c>
+      <c r="F26" s="65">
+        <v>9</v>
+      </c>
+      <c r="G26" s="65">
+        <v>20</v>
+      </c>
+      <c r="H26" s="65">
+        <v>8</v>
+      </c>
+      <c r="I26" s="65">
+        <v>270</v>
+      </c>
+      <c r="J26" s="65">
+        <v>270</v>
+      </c>
+      <c r="K26" s="66">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -8519,14 +8836,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>9</v>
+      </c>
+      <c r="E27" s="62">
+        <v>17</v>
+      </c>
+      <c r="F27" s="62">
+        <v>52</v>
+      </c>
+      <c r="G27" s="62">
+        <v>9</v>
+      </c>
+      <c r="H27" s="62">
+        <v>31</v>
+      </c>
+      <c r="I27" s="62">
+        <v>30</v>
+      </c>
+      <c r="J27" s="62">
+        <v>15</v>
+      </c>
+      <c r="K27" s="63">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -8534,14 +8867,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>61</v>
+      </c>
+      <c r="E28" s="65">
+        <v>48</v>
+      </c>
+      <c r="F28" s="65">
+        <v>68</v>
+      </c>
+      <c r="G28" s="65">
+        <v>60</v>
+      </c>
+      <c r="H28" s="65">
+        <v>69</v>
+      </c>
+      <c r="I28" s="65">
+        <v>2</v>
+      </c>
+      <c r="J28" s="65">
+        <v>2</v>
+      </c>
+      <c r="K28" s="66">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -8551,14 +8900,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>61</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16">
+        <v>132</v>
+      </c>
+      <c r="G29" s="16">
+        <v>126</v>
+      </c>
+      <c r="H29" s="16">
+        <v>144</v>
+      </c>
+      <c r="I29" s="16">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16">
+        <v>10</v>
+      </c>
+      <c r="K29" s="68">
+        <v>113</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -8566,14 +8931,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>65</v>
+      </c>
+      <c r="E30" s="65">
+        <v>270</v>
+      </c>
+      <c r="F30" s="65">
+        <v>35</v>
+      </c>
+      <c r="G30" s="65">
+        <v>270</v>
+      </c>
+      <c r="H30" s="65">
+        <v>23</v>
+      </c>
+      <c r="I30" s="65">
+        <v>2</v>
+      </c>
+      <c r="J30" s="65">
+        <v>33</v>
+      </c>
+      <c r="K30" s="66">
+        <v>143</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -8758,7 +9139,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8766,29 +9147,26 @@
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9384,28 +9762,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>25.1</v>
+      </c>
+      <c r="E23" s="62">
+        <v>53.29</v>
+      </c>
+      <c r="F23" s="62">
+        <v>41.11</v>
+      </c>
+      <c r="G23" s="62">
+        <v>34.81</v>
+      </c>
+      <c r="H23" s="62">
+        <v>42.07</v>
+      </c>
+      <c r="I23" s="62">
+        <v>249.14</v>
+      </c>
+      <c r="J23" s="62">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="K23" s="63">
+        <v>20.66</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>19.59</v>
+      </c>
+      <c r="E24" s="65">
+        <v>26.52</v>
+      </c>
+      <c r="F24" s="65">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="G24" s="65">
+        <v>14.27</v>
+      </c>
+      <c r="H24" s="65">
+        <v>12.94</v>
+      </c>
+      <c r="I24" s="65">
+        <v>95.14</v>
+      </c>
+      <c r="J24" s="65">
+        <v>15.32</v>
+      </c>
+      <c r="K24" s="66">
+        <v>34.72</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -9415,28 +9825,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>19.38</v>
+      </c>
+      <c r="E25" s="62">
+        <v>5.61</v>
+      </c>
+      <c r="F25" s="62">
+        <v>85.97</v>
+      </c>
+      <c r="G25" s="62">
+        <v>48.64</v>
+      </c>
+      <c r="H25" s="62">
+        <v>45.63</v>
+      </c>
+      <c r="I25" s="62">
+        <v>270</v>
+      </c>
+      <c r="J25" s="62">
+        <v>56.38</v>
+      </c>
+      <c r="K25" s="63">
+        <v>24.38</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="E26" s="65">
+        <v>33.770000000000003</v>
+      </c>
+      <c r="F26" s="65">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="G26" s="65">
+        <v>19.61</v>
+      </c>
+      <c r="H26" s="65">
+        <v>7.81</v>
+      </c>
+      <c r="I26" s="65">
+        <v>270</v>
+      </c>
+      <c r="J26" s="65">
+        <v>270</v>
+      </c>
+      <c r="K26" s="66">
+        <v>19.670000000000002</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -9446,14 +9888,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>11.18</v>
+      </c>
+      <c r="E27" s="62">
+        <v>19.78</v>
+      </c>
+      <c r="F27" s="62">
+        <v>48.55</v>
+      </c>
+      <c r="G27" s="62">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="H27" s="62">
+        <v>40.65</v>
+      </c>
+      <c r="I27" s="62">
+        <v>25.5</v>
+      </c>
+      <c r="J27" s="62">
+        <v>16.39</v>
+      </c>
+      <c r="K27" s="63">
+        <v>50.75</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -9461,14 +9919,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>51.94</v>
+      </c>
+      <c r="E28" s="65">
+        <v>50.53</v>
+      </c>
+      <c r="F28" s="65">
+        <v>58.43</v>
+      </c>
+      <c r="G28" s="65">
+        <v>57.68</v>
+      </c>
+      <c r="H28" s="65">
+        <v>56.11</v>
+      </c>
+      <c r="I28" s="65">
+        <v>2</v>
+      </c>
+      <c r="J28" s="65">
+        <v>2</v>
+      </c>
+      <c r="K28" s="66">
+        <v>53.38</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -9478,14 +9952,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>62.26</v>
+      </c>
+      <c r="E29" s="16">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16">
+        <v>151.80000000000001</v>
+      </c>
+      <c r="G29" s="16">
+        <v>129.51</v>
+      </c>
+      <c r="H29" s="16">
+        <v>136.63999999999999</v>
+      </c>
+      <c r="I29" s="16">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="K29" s="68">
+        <v>104.59</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -9493,14 +9983,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>61.49</v>
+      </c>
+      <c r="E30" s="65">
+        <v>270</v>
+      </c>
+      <c r="F30" s="65">
+        <v>36.32</v>
+      </c>
+      <c r="G30" s="65">
+        <v>270</v>
+      </c>
+      <c r="H30" s="65">
+        <v>27.63</v>
+      </c>
+      <c r="I30" s="65">
+        <v>2</v>
+      </c>
+      <c r="J30" s="65">
+        <v>30.91</v>
+      </c>
+      <c r="K30" s="66">
+        <v>125.82</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -9685,7 +10191,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9694,8 +10200,9 @@
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
@@ -9703,19 +10210,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10311,28 +10818,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>2</v>
+      </c>
+      <c r="E23" s="62">
+        <v>10</v>
+      </c>
+      <c r="F23" s="62">
+        <v>4</v>
+      </c>
+      <c r="G23" s="62">
+        <v>1</v>
+      </c>
+      <c r="H23" s="62">
+        <v>1</v>
+      </c>
+      <c r="I23" s="62">
+        <v>7</v>
+      </c>
+      <c r="J23" s="62">
+        <v>4</v>
+      </c>
+      <c r="K23" s="63">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>7</v>
+      </c>
+      <c r="E24" s="65">
+        <v>5</v>
+      </c>
+      <c r="F24" s="65">
+        <v>3</v>
+      </c>
+      <c r="G24" s="65">
+        <v>9</v>
+      </c>
+      <c r="H24" s="65">
+        <v>10</v>
+      </c>
+      <c r="I24" s="65">
+        <v>5</v>
+      </c>
+      <c r="J24" s="65">
+        <v>9</v>
+      </c>
+      <c r="K24" s="66">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -10342,28 +10881,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>6</v>
+      </c>
+      <c r="E25" s="62">
+        <v>1</v>
+      </c>
+      <c r="F25" s="62">
+        <v>9</v>
+      </c>
+      <c r="G25" s="62">
+        <v>10</v>
+      </c>
+      <c r="H25" s="62">
+        <v>7</v>
+      </c>
+      <c r="I25" s="62">
+        <v>5</v>
+      </c>
+      <c r="J25" s="62">
+        <v>6</v>
+      </c>
+      <c r="K25" s="63">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>7</v>
+      </c>
+      <c r="E26" s="65">
+        <v>8</v>
+      </c>
+      <c r="F26" s="65">
+        <v>1</v>
+      </c>
+      <c r="G26" s="65">
+        <v>1</v>
+      </c>
+      <c r="H26" s="65">
+        <v>1</v>
+      </c>
+      <c r="I26" s="65">
+        <v>2</v>
+      </c>
+      <c r="J26" s="65">
+        <v>1</v>
+      </c>
+      <c r="K26" s="66">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -10373,14 +10944,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>3</v>
+      </c>
+      <c r="E27" s="62">
+        <v>7</v>
+      </c>
+      <c r="F27" s="62">
+        <v>9</v>
+      </c>
+      <c r="G27" s="62">
+        <v>9</v>
+      </c>
+      <c r="H27" s="62">
+        <v>1</v>
+      </c>
+      <c r="I27" s="62">
+        <v>7</v>
+      </c>
+      <c r="J27" s="62">
+        <v>6</v>
+      </c>
+      <c r="K27" s="63">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -10388,14 +10975,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>6</v>
+      </c>
+      <c r="E28" s="65">
+        <v>1</v>
+      </c>
+      <c r="F28" s="65">
+        <v>2</v>
+      </c>
+      <c r="G28" s="65">
+        <v>1</v>
+      </c>
+      <c r="H28" s="65">
+        <v>1</v>
+      </c>
+      <c r="I28" s="65">
+        <v>3</v>
+      </c>
+      <c r="J28" s="65">
+        <v>1</v>
+      </c>
+      <c r="K28" s="66">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -10405,14 +11008,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>6</v>
+      </c>
+      <c r="E29" s="16">
+        <v>10</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+      <c r="G29" s="16">
+        <v>10</v>
+      </c>
+      <c r="H29" s="16">
+        <v>9</v>
+      </c>
+      <c r="I29" s="16">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16">
+        <v>7</v>
+      </c>
+      <c r="K29" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -10420,14 +11039,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>9</v>
+      </c>
+      <c r="E30" s="65">
+        <v>1</v>
+      </c>
+      <c r="F30" s="65">
+        <v>4</v>
+      </c>
+      <c r="G30" s="65">
+        <v>1</v>
+      </c>
+      <c r="H30" s="65">
+        <v>3</v>
+      </c>
+      <c r="I30" s="65">
+        <v>6</v>
+      </c>
+      <c r="J30" s="65">
+        <v>1</v>
+      </c>
+      <c r="K30" s="66">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -10612,7 +11247,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10621,8 +11256,9 @@
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
@@ -10630,19 +11266,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11238,28 +11874,60 @@
         <v>1</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
+      <c r="D23" s="61">
+        <v>2</v>
+      </c>
+      <c r="E23" s="62">
+        <v>10</v>
+      </c>
+      <c r="F23" s="62">
+        <v>4</v>
+      </c>
+      <c r="G23" s="62">
+        <v>1</v>
+      </c>
+      <c r="H23" s="62">
+        <v>1</v>
+      </c>
+      <c r="I23" s="62">
+        <v>7</v>
+      </c>
+      <c r="J23" s="62">
+        <v>4</v>
+      </c>
+      <c r="K23" s="63">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="72"/>
+      <c r="D24" s="64">
+        <v>7</v>
+      </c>
+      <c r="E24" s="65">
+        <v>5</v>
+      </c>
+      <c r="F24" s="65">
+        <v>3</v>
+      </c>
+      <c r="G24" s="65">
+        <v>9</v>
+      </c>
+      <c r="H24" s="65">
+        <v>10</v>
+      </c>
+      <c r="I24" s="65">
+        <v>5</v>
+      </c>
+      <c r="J24" s="65">
+        <v>9</v>
+      </c>
+      <c r="K24" s="66">
+        <v>9</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -11269,28 +11937,60 @@
         <v>1</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="68"/>
-      <c r="H25" s="68"/>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
+      <c r="D25" s="61">
+        <v>6</v>
+      </c>
+      <c r="E25" s="62">
+        <v>1</v>
+      </c>
+      <c r="F25" s="62">
+        <v>9</v>
+      </c>
+      <c r="G25" s="62">
+        <v>10</v>
+      </c>
+      <c r="H25" s="62">
+        <v>7</v>
+      </c>
+      <c r="I25" s="62">
+        <v>5</v>
+      </c>
+      <c r="J25" s="62">
+        <v>6</v>
+      </c>
+      <c r="K25" s="63">
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="72"/>
+      <c r="D26" s="64">
+        <v>7</v>
+      </c>
+      <c r="E26" s="65">
+        <v>8</v>
+      </c>
+      <c r="F26" s="65">
+        <v>1</v>
+      </c>
+      <c r="G26" s="65">
+        <v>1</v>
+      </c>
+      <c r="H26" s="65">
+        <v>1</v>
+      </c>
+      <c r="I26" s="65">
+        <v>2</v>
+      </c>
+      <c r="J26" s="65">
+        <v>1</v>
+      </c>
+      <c r="K26" s="66">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -11300,14 +12000,30 @@
         <v>1</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="69"/>
+      <c r="D27" s="61">
+        <v>3</v>
+      </c>
+      <c r="E27" s="62">
+        <v>7</v>
+      </c>
+      <c r="F27" s="62">
+        <v>9</v>
+      </c>
+      <c r="G27" s="62">
+        <v>9</v>
+      </c>
+      <c r="H27" s="62">
+        <v>1</v>
+      </c>
+      <c r="I27" s="62">
+        <v>7</v>
+      </c>
+      <c r="J27" s="62">
+        <v>6</v>
+      </c>
+      <c r="K27" s="63">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
@@ -11315,14 +12031,30 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="72"/>
+      <c r="D28" s="64">
+        <v>6</v>
+      </c>
+      <c r="E28" s="65">
+        <v>1</v>
+      </c>
+      <c r="F28" s="65">
+        <v>2</v>
+      </c>
+      <c r="G28" s="65">
+        <v>1</v>
+      </c>
+      <c r="H28" s="65">
+        <v>1</v>
+      </c>
+      <c r="I28" s="65">
+        <v>3</v>
+      </c>
+      <c r="J28" s="65">
+        <v>1</v>
+      </c>
+      <c r="K28" s="66">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
@@ -11332,14 +12064,30 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="74"/>
+      <c r="D29" s="67">
+        <v>6</v>
+      </c>
+      <c r="E29" s="16">
+        <v>10</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+      <c r="G29" s="16">
+        <v>10</v>
+      </c>
+      <c r="H29" s="16">
+        <v>9</v>
+      </c>
+      <c r="I29" s="16">
+        <v>1</v>
+      </c>
+      <c r="J29" s="16">
+        <v>7</v>
+      </c>
+      <c r="K29" s="68">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
@@ -11347,14 +12095,30 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
+      <c r="D30" s="64">
+        <v>9</v>
+      </c>
+      <c r="E30" s="65">
+        <v>1</v>
+      </c>
+      <c r="F30" s="65">
+        <v>4</v>
+      </c>
+      <c r="G30" s="65">
+        <v>1</v>
+      </c>
+      <c r="H30" s="65">
+        <v>3</v>
+      </c>
+      <c r="I30" s="65">
+        <v>6</v>
+      </c>
+      <c r="J30" s="65">
+        <v>1</v>
+      </c>
+      <c r="K30" s="66">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
@@ -11562,24 +12326,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11589,29 +12353,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="63" t="s">
+      <c r="L3" s="72"/>
+      <c r="M3" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="64"/>
-      <c r="O3" s="63" t="s">
+      <c r="N3" s="72"/>
+      <c r="O3" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="65"/>
+      <c r="P3" s="73"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">

</xml_diff>

<commit_message>
started highlighting best accuracies of each line
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D07E79-9012-4CCD-8B55-5EAFF121ECC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2AE590-9ECB-45C9-B2B6-4923CC08AD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5039,8 +5039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4BD5FD7-7F47-465E-A9A3-1FAE665B7AD8}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
small correction in cervCancer results
</commit_message>
<xml_diff>
--- a/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
+++ b/results_analysis/spark_cervicalCancer_02_hold_02_best.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CF313A-0A2A-4A9A-B0BC-96521F29305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BD29A6-E23C-44D0-A2CD-46DE586732F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_mean" sheetId="1" r:id="rId1"/>
@@ -743,24 +743,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,6 +762,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,19 +1084,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1704,10 +1704,10 @@
       <c r="D23" s="61">
         <v>0.87633851468048396</v>
       </c>
-      <c r="E23" s="75">
+      <c r="E23" s="69">
         <v>0.89400690846286701</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="69">
         <v>0.89162348877374797</v>
       </c>
       <c r="G23" s="62">
@@ -1716,7 +1716,7 @@
       <c r="H23" s="62">
         <v>0.83075993091537104</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="69">
         <v>0.90312607944732304</v>
       </c>
       <c r="J23" s="62">
@@ -1731,7 +1731,7 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="D24" s="77">
+      <c r="D24" s="71">
         <v>0.89388601036269399</v>
       </c>
       <c r="E24" s="65">
@@ -1746,10 +1746,10 @@
       <c r="H24" s="65">
         <v>0.80283246977547496</v>
       </c>
-      <c r="I24" s="76">
+      <c r="I24" s="70">
         <v>0.938791018998273</v>
       </c>
-      <c r="J24" s="76">
+      <c r="J24" s="70">
         <v>0.90037996545768595</v>
       </c>
       <c r="K24" s="66">
@@ -1770,7 +1770,7 @@
       <c r="E25" s="62">
         <v>0.76649395509499096</v>
       </c>
-      <c r="F25" s="75">
+      <c r="F25" s="69">
         <v>0.90469775474956804</v>
       </c>
       <c r="G25" s="62">
@@ -1779,10 +1779,10 @@
       <c r="H25" s="62">
         <v>0.87853195164076003</v>
       </c>
-      <c r="I25" s="75">
+      <c r="I25" s="69">
         <v>0.92369602763385195</v>
       </c>
-      <c r="J25" s="75">
+      <c r="J25" s="69">
         <v>0.91958549222797903</v>
       </c>
       <c r="K25" s="63">
@@ -1794,7 +1794,7 @@
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="D26" s="77">
+      <c r="D26" s="71">
         <v>0.90796200345423095</v>
       </c>
       <c r="E26" s="65">
@@ -1809,10 +1809,10 @@
       <c r="H26" s="65">
         <v>0.76785837651122602</v>
       </c>
-      <c r="I26" s="76">
+      <c r="I26" s="70">
         <v>0.90302245250431801</v>
       </c>
-      <c r="J26" s="76">
+      <c r="J26" s="70">
         <v>0.90390328151986199</v>
       </c>
       <c r="K26" s="66">
@@ -1833,7 +1833,7 @@
       <c r="E27" s="62">
         <v>0.86215889464594098</v>
       </c>
-      <c r="F27" s="75">
+      <c r="F27" s="69">
         <v>0.87861830742659797</v>
       </c>
       <c r="G27" s="62">
@@ -1842,13 +1842,13 @@
       <c r="H27" s="62">
         <v>0.84929188255613097</v>
       </c>
-      <c r="I27" s="75">
+      <c r="I27" s="69">
         <v>0.87062176165803096</v>
       </c>
       <c r="J27" s="62">
         <v>0.85457685664939498</v>
       </c>
-      <c r="K27" s="78">
+      <c r="K27" s="72">
         <v>0.88113989637305701</v>
       </c>
     </row>
@@ -1858,16 +1858,16 @@
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="77">
+      <c r="D28" s="71">
         <v>0.87278065630397195</v>
       </c>
       <c r="E28" s="65">
         <v>0.84659758203799695</v>
       </c>
-      <c r="F28" s="65">
+      <c r="F28" s="70">
         <v>0.84785837651122598</v>
       </c>
-      <c r="G28" s="65">
+      <c r="G28" s="70">
         <v>0.84816925734024196</v>
       </c>
       <c r="H28" s="65">
@@ -1879,7 +1879,7 @@
       <c r="J28" s="65">
         <v>0.78910189982728796</v>
       </c>
-      <c r="K28" s="79">
+      <c r="K28" s="73">
         <v>0.86214162348877399</v>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="80">
+      <c r="D29" s="74">
         <v>0.92203799654576901</v>
       </c>
       <c r="E29" s="16">
@@ -1900,10 +1900,10 @@
       <c r="F29" s="16">
         <v>0.89070811744386902</v>
       </c>
-      <c r="G29" s="81">
+      <c r="G29" s="75">
         <v>0.91837651122625197</v>
       </c>
-      <c r="H29" s="81">
+      <c r="H29" s="75">
         <v>0.91870466321243505</v>
       </c>
       <c r="I29" s="16">
@@ -1922,16 +1922,16 @@
         <v>2</v>
       </c>
       <c r="C30" s="6"/>
-      <c r="D30" s="77">
+      <c r="D30" s="71">
         <v>0.92295336787564797</v>
       </c>
-      <c r="E30" s="76">
+      <c r="E30" s="70">
         <v>0.903747841105354</v>
       </c>
       <c r="F30" s="65">
         <v>0.89053540587219304</v>
       </c>
-      <c r="G30" s="76">
+      <c r="G30" s="70">
         <v>0.90041450777202103</v>
       </c>
       <c r="H30" s="65">
@@ -1943,7 +1943,7 @@
       <c r="J30" s="65">
         <v>0.84428324697754698</v>
       </c>
-      <c r="K30" s="79">
+      <c r="K30" s="73">
         <v>0.913333333333333</v>
       </c>
     </row>
@@ -2182,6 +2182,7 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2211,61 +2212,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="72"/>
-      <c r="F3" s="71" t="s">
+      <c r="E3" s="79"/>
+      <c r="F3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="71" t="s">
+      <c r="G3" s="79"/>
+      <c r="H3" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="72"/>
-      <c r="J3" s="71" t="s">
+      <c r="I3" s="79"/>
+      <c r="J3" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="72"/>
-      <c r="L3" s="71" t="s">
+      <c r="K3" s="79"/>
+      <c r="L3" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="72"/>
-      <c r="N3" s="71" t="s">
+      <c r="M3" s="79"/>
+      <c r="N3" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="72"/>
-      <c r="P3" s="71" t="s">
+      <c r="O3" s="79"/>
+      <c r="P3" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="71" t="s">
+      <c r="Q3" s="79"/>
+      <c r="R3" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="73"/>
+      <c r="S3" s="80"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -3550,19 +3551,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4315,19 +4316,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5087,19 +5088,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6211,19 +6212,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7138,19 +7139,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8131,19 +8132,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9183,19 +9184,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -10239,19 +10240,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -11295,19 +11296,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12355,24 +12356,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12382,29 +12383,29 @@
       <c r="E3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="F3" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
       <c r="I3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="71" t="s">
+      <c r="K3" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="71" t="s">
+      <c r="L3" s="79"/>
+      <c r="M3" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="71" t="s">
+      <c r="N3" s="79"/>
+      <c r="O3" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="73"/>
+      <c r="P3" s="80"/>
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">

</xml_diff>